<commit_message>
add statistics june sizod
</commit_message>
<xml_diff>
--- a/kaskad/production/sizod/zeh3linii/statistics-full.xlsx
+++ b/kaskad/production/sizod/zeh3linii/statistics-full.xlsx
@@ -717,6 +717,12 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -821,12 +827,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1142,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M29"/>
+  <dimension ref="A2:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,13 +1166,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="56"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1181,13 +1181,13 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1199,12 +1199,12 @@
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="77"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1217,12 +1217,12 @@
       <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="74"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="76"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1235,12 +1235,12 @@
       <c r="A6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="71"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="73"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1253,12 +1253,12 @@
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="68"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="70"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1271,12 +1271,12 @@
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="65"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1289,12 +1289,12 @@
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1305,10 +1305,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1341,36 +1341,36 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="82"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="84"/>
     </row>
     <row r="14" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="58"/>
-      <c r="B14" s="55" t="s">
+      <c r="A14" s="60"/>
+      <c r="B14" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="55" t="s">
+      <c r="C14" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="85" t="s">
+      <c r="D14" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="57" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="40" t="s">
@@ -1391,19 +1391,19 @@
       <c r="K14" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="50" t="s">
+      <c r="L14" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="83" t="s">
+      <c r="M14" s="85" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="59"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="56"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="58"/>
       <c r="F15" s="14" t="s">
         <v>10</v>
       </c>
@@ -1422,8 +1422,8 @@
       <c r="K15" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="51"/>
-      <c r="M15" s="84"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="86"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="49">
@@ -1704,63 +1704,104 @@
       </c>
       <c r="M22" s="48"/>
     </row>
-    <row r="23" spans="1:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
+    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49">
+        <v>45444</v>
+      </c>
+      <c r="B23" s="9">
+        <v>3.16</v>
+      </c>
+      <c r="C23" s="10">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>3.49</v>
+      </c>
+      <c r="F23" s="37">
+        <v>0</v>
+      </c>
+      <c r="G23" s="27">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H23" s="18">
+        <v>3.2370000000000001</v>
+      </c>
+      <c r="I23" s="28">
+        <v>0.16</v>
+      </c>
+      <c r="J23" s="29">
+        <v>0.16</v>
+      </c>
+      <c r="K23" s="30">
+        <v>2.7229999999999999</v>
+      </c>
+      <c r="L23" s="24">
+        <f>SUM(B23,C23,D23,E23,F23,G23,H23,I23,J23,K23)</f>
+        <v>17.152999999999999</v>
+      </c>
+      <c r="M23" s="48"/>
+    </row>
+    <row r="24" spans="1:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="35">
-        <f>SUM(B16:B22)</f>
+      <c r="B24" s="35">
+        <f t="shared" ref="B24:L24" si="1">SUM(B16:B22)</f>
         <v>17.082999999999998</v>
       </c>
-      <c r="C23" s="34">
-        <f>SUM(C16:C22)</f>
+      <c r="C24" s="34">
+        <f t="shared" si="1"/>
         <v>17.056000000000001</v>
       </c>
-      <c r="D23" s="36">
-        <f>SUM(D16:D22)</f>
+      <c r="D24" s="36">
+        <f t="shared" si="1"/>
         <v>77.328999999999994</v>
       </c>
-      <c r="E23" s="36">
-        <f>SUM(E16:E22)</f>
+      <c r="E24" s="36">
+        <f t="shared" si="1"/>
         <v>7.6400000000000006</v>
       </c>
-      <c r="F23" s="46">
-        <f>SUM(F16:F22)</f>
+      <c r="F24" s="46">
+        <f t="shared" si="1"/>
         <v>5.25</v>
       </c>
-      <c r="G23" s="46">
-        <f>SUM(G16:G22)</f>
+      <c r="G24" s="46">
+        <f t="shared" si="1"/>
         <v>0.90300000000000002</v>
       </c>
-      <c r="H23" s="45">
-        <f>SUM(H16:H22)</f>
+      <c r="H24" s="45">
+        <f t="shared" si="1"/>
         <v>20.107000000000003</v>
       </c>
-      <c r="I23" s="45">
-        <f>SUM(I16:I22)</f>
+      <c r="I24" s="45">
+        <f t="shared" si="1"/>
         <v>31.328000000000003</v>
       </c>
-      <c r="J23" s="45">
-        <f>SUM(J16:J22)</f>
+      <c r="J24" s="45">
+        <f t="shared" si="1"/>
         <v>5.3100000000000005</v>
       </c>
-      <c r="K23" s="42">
-        <f>SUM(K16:K22)</f>
+      <c r="K24" s="42">
+        <f t="shared" si="1"/>
         <v>50.462999999999994</v>
       </c>
-      <c r="L23" s="35">
-        <f>SUM(L16:L22)</f>
+      <c r="L24" s="35">
+        <f t="shared" si="1"/>
         <v>232.87799999999996</v>
       </c>
-      <c r="M23" s="47"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K29" t="s">
+      <c r="M24" s="47"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="M14:M15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="A2:E2"/>
@@ -1777,7 +1818,6 @@
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B13:M13"/>
-    <mergeCell ref="M14:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add graphics sushilki, gorelki. Small fixes
</commit_message>
<xml_diff>
--- a/kaskad/production/sizod/zeh3linii/statistics-full.xlsx
+++ b/kaskad/production/sizod/zeh3linii/statistics-full.xlsx
@@ -766,12 +766,96 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -792,90 +876,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1194,7 +1194,7 @@
   <dimension ref="A2:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,13 +1215,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="78"/>
+      <c r="A2" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="69"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1230,13 +1230,13 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1248,12 +1248,12 @@
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="99"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1266,12 +1266,12 @@
       <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="96"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1284,12 +1284,12 @@
       <c r="A6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1302,12 +1302,12 @@
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="90"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="83"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1320,12 +1320,12 @@
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="87"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1338,12 +1338,12 @@
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="84"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1354,10 +1354,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1390,36 +1390,36 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
-      <c r="M13" s="69"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="96"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="97"/>
     </row>
     <row r="14" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="80"/>
-      <c r="B14" s="65" t="s">
+      <c r="A14" s="73"/>
+      <c r="B14" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="72" t="s">
+      <c r="D14" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="70" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="39" t="s">
@@ -1440,19 +1440,19 @@
       <c r="K14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="70" t="s">
+      <c r="M14" s="98" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="66"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="71"/>
       <c r="F15" s="14" t="s">
         <v>10</v>
       </c>
@@ -1471,8 +1471,8 @@
       <c r="K15" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="75"/>
-      <c r="M15" s="71"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="99"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
@@ -1708,7 +1708,7 @@
         <v>2.456</v>
       </c>
       <c r="L21" s="24">
-        <f>SUM(B21,C21,D21,E21,F21,G21,H21,I21,J21,K21)</f>
+        <f t="shared" ref="L21:L26" si="1">SUM(B21,C21,D21,E21,F21,G21,H21,I21,J21,K21)</f>
         <v>11.760999999999999</v>
       </c>
       <c r="M21" s="43"/>
@@ -1748,7 +1748,7 @@
         <v>15.446</v>
       </c>
       <c r="L22" s="24">
-        <f>SUM(B22,C22,D22,E22,F22,G22,H22,I22,J22,K22)</f>
+        <f t="shared" si="1"/>
         <v>26.963999999999999</v>
       </c>
       <c r="M22" s="43"/>
@@ -1788,7 +1788,7 @@
         <v>2.7229999999999999</v>
       </c>
       <c r="L23" s="54">
-        <f>SUM(B23,C23,D23,E23,F23,G23,H23,I23,J23,K23)</f>
+        <f t="shared" si="1"/>
         <v>17.152999999999999</v>
       </c>
       <c r="M23" s="55"/>
@@ -1828,7 +1828,7 @@
         <v>8.6</v>
       </c>
       <c r="L24" s="63">
-        <f>SUM(B24,C24,D24,E24,F24,G24,H24,I24,J24,K24)</f>
+        <f t="shared" si="1"/>
         <v>18.393000000000001</v>
       </c>
       <c r="M24" s="64"/>
@@ -1868,7 +1868,7 @@
         <v>3.74</v>
       </c>
       <c r="L25" s="63">
-        <f>SUM(B25,C25,D25,E25,F25,G25,H25,I25,J25,K25)</f>
+        <f t="shared" si="1"/>
         <v>16.042999999999999</v>
       </c>
       <c r="M25" s="64"/>
@@ -1908,10 +1908,50 @@
         <v>5.36</v>
       </c>
       <c r="L26" s="63">
-        <f>SUM(B26,C26,D26,E26,F26,G26,H26,I26,J26,K26)</f>
+        <f t="shared" si="1"/>
         <v>19.365000000000002</v>
       </c>
       <c r="M26" s="64"/>
+    </row>
+    <row r="27" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="56">
+        <v>45566</v>
+      </c>
+      <c r="B27" s="33">
+        <v>0</v>
+      </c>
+      <c r="C27" s="33">
+        <v>3.49</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0</v>
+      </c>
+      <c r="E27" s="33">
+        <v>2</v>
+      </c>
+      <c r="F27" s="57">
+        <v>0</v>
+      </c>
+      <c r="G27" s="58">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="H27" s="59">
+        <v>6.22</v>
+      </c>
+      <c r="I27" s="60">
+        <v>2.84</v>
+      </c>
+      <c r="J27" s="61">
+        <v>0</v>
+      </c>
+      <c r="K27" s="62">
+        <v>1.7529999999999999</v>
+      </c>
+      <c r="L27" s="63">
+        <f t="shared" ref="L27" si="2">SUM(B27,C27,D27,E27,F27,G27,H27,I27,J27,K27)</f>
+        <v>16.545999999999999</v>
+      </c>
+      <c r="M27" s="64"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K30" t="s">
@@ -1920,6 +1960,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="L14:L15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="A13:A15"/>
@@ -1935,8 +1977,6 @@
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="M14:M15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="L14:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
statistics dot-eko, graph vr sorted
</commit_message>
<xml_diff>
--- a/kaskad/production/sizod/zeh3linii/statistics-full.xlsx
+++ b/kaskad/production/sizod/zeh3linii/statistics-full.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -110,13 +110,13 @@
     <t>общая</t>
   </si>
   <si>
-    <t>2023-2024</t>
-  </si>
-  <si>
     <t>Месяц</t>
   </si>
   <si>
     <t xml:space="preserve">Итого простоя </t>
+  </si>
+  <si>
+    <t>2023-2025</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,15 +593,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,7 +644,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -763,6 +763,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -841,7 +853,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -856,22 +868,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1188,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M30"/>
+  <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,13 +1209,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
+      <c r="A2" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="71"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1227,13 +1224,13 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1245,12 +1242,12 @@
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="90"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="94"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1263,12 +1260,12 @@
       <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="87"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="91"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1281,12 +1278,12 @@
       <c r="A6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="84"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1299,12 +1296,12 @@
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="81"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="85"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1317,12 +1314,12 @@
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="78"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="82"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1335,12 +1332,12 @@
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="75"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="79"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1351,10 +1348,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1380,43 +1377,43 @@
         <v>24</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="93" t="s">
+      <c r="A13" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="95"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="99"/>
     </row>
     <row r="14" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="71"/>
-      <c r="B14" s="68" t="s">
+      <c r="A14" s="75"/>
+      <c r="B14" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="68" t="s">
+      <c r="E14" s="72" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="39" t="s">
@@ -1437,19 +1434,19 @@
       <c r="K14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="96" t="s">
+      <c r="L14" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="100" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="72"/>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="69"/>
+      <c r="A15" s="76"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="14" t="s">
         <v>10</v>
       </c>
@@ -1468,8 +1465,8 @@
       <c r="K15" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="101"/>
-      <c r="M15" s="97"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="73"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
@@ -1985,7 +1982,7 @@
         <v>3.8</v>
       </c>
       <c r="L28" s="63">
-        <f t="shared" ref="L28:L30" si="3">SUM(B28,C28,D28,E28,F28,G28,H28,I28,J28,K28)</f>
+        <f t="shared" ref="L28" si="3">SUM(B28,C28,D28,E28,F28,G28,H28,I28,J28,K28)</f>
         <v>16.419999999999998</v>
       </c>
       <c r="M28" s="64"/>
@@ -2068,8 +2065,49 @@
       </c>
       <c r="M30" s="64"/>
     </row>
+    <row r="31" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="56">
+        <v>45689</v>
+      </c>
+      <c r="B31" s="34">
+        <v>0</v>
+      </c>
+      <c r="C31" s="33">
+        <v>0.24</v>
+      </c>
+      <c r="D31" s="35">
+        <v>0</v>
+      </c>
+      <c r="E31" s="35">
+        <v>3.91</v>
+      </c>
+      <c r="F31" s="57">
+        <v>0.41</v>
+      </c>
+      <c r="G31" s="58">
+        <v>0</v>
+      </c>
+      <c r="H31" s="59">
+        <v>2.57</v>
+      </c>
+      <c r="I31" s="60">
+        <v>0.82</v>
+      </c>
+      <c r="J31" s="61">
+        <v>0</v>
+      </c>
+      <c r="K31" s="62">
+        <v>5.52</v>
+      </c>
+      <c r="L31" s="63">
+        <v>13.47</v>
+      </c>
+      <c r="M31" s="64"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="D14:D15"/>
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="C14:C15"/>
@@ -2085,8 +2123,6 @@
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B13:M13"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="D14:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add march2025 doeko statistic + 2 video instruction
</commit_message>
<xml_diff>
--- a/kaskad/production/sizod/zeh3linii/statistics-full.xlsx
+++ b/kaskad/production/sizod/zeh3linii/statistics-full.xlsx
@@ -763,6 +763,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -787,9 +793,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -867,9 +870,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1185,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M31"/>
+  <dimension ref="A2:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,13 +1209,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
+      <c r="A2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1224,13 +1224,13 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1242,12 +1242,12 @@
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="95"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1260,12 +1260,12 @@
       <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1278,12 +1278,12 @@
       <c r="A6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="89"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1296,12 +1296,12 @@
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1314,12 +1314,12 @@
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1332,12 +1332,12 @@
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="80"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1348,10 +1348,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1384,36 +1384,36 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="99"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="100"/>
     </row>
     <row r="14" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="75"/>
-      <c r="B14" s="72" t="s">
+      <c r="A14" s="76"/>
+      <c r="B14" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="74" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="39" t="s">
@@ -1434,19 +1434,19 @@
       <c r="K14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="67" t="s">
+      <c r="L14" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="M14" s="100" t="s">
+      <c r="M14" s="65" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="76"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="73"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="66"/>
       <c r="F15" s="14" t="s">
         <v>10</v>
       </c>
@@ -1465,8 +1465,8 @@
       <c r="K15" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="68"/>
-      <c r="M15" s="73"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="66"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
@@ -2104,8 +2104,48 @@
       </c>
       <c r="M31" s="64"/>
     </row>
+    <row r="32" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="56">
+        <v>45717</v>
+      </c>
+      <c r="B32" s="34">
+        <v>0</v>
+      </c>
+      <c r="C32" s="33">
+        <v>0</v>
+      </c>
+      <c r="D32" s="35">
+        <v>0</v>
+      </c>
+      <c r="E32" s="35">
+        <v>0</v>
+      </c>
+      <c r="F32" s="57">
+        <v>0</v>
+      </c>
+      <c r="G32" s="58">
+        <v>0</v>
+      </c>
+      <c r="H32" s="59">
+        <v>5.8</v>
+      </c>
+      <c r="I32" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="J32" s="61">
+        <v>0</v>
+      </c>
+      <c r="K32" s="62">
+        <v>1</v>
+      </c>
+      <c r="L32" s="63">
+        <v>7.3</v>
+      </c>
+      <c r="M32" s="64"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B13:M13"/>
     <mergeCell ref="M14:M15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="L14:L15"/>
@@ -2122,7 +2162,6 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B13:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>